<commit_message>
Add items to Gantt Chart
</commit_message>
<xml_diff>
--- a/Projektplan.xlsx
+++ b/Projektplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\HSR\Module\_BA\Dokumente\BA-Projektplan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gubi/Documents/BA/BA-Projektplan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B483566B-4A98-4C70-82A7-24E306E916A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C36D295-DB3A-F04B-B7EC-6DBA2AD8999D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplan" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>TASK NAME</t>
   </si>
@@ -51,9 +51,6 @@
     <t>DURATION* (WORK DAYS)</t>
   </si>
   <si>
-    <t>Detailkonzept</t>
-  </si>
-  <si>
     <t>Infrastruktur einrichten</t>
   </si>
   <si>
@@ -127,6 +124,12 @@
   </si>
   <si>
     <t>Bugfixes</t>
+  </si>
+  <si>
+    <t>Datenbankschema planen</t>
+  </si>
+  <si>
+    <t>Sequenzdiagramme erstellt</t>
   </si>
 </sst>
 </file>
@@ -297,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -364,16 +367,17 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +398,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -416,9 +420,9 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>Projektplan!$B$9:$B$33</c:f>
+              <c:f>Projektplan!$B$9:$B$34</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>M0: Kickoff</c:v>
                 </c:pt>
@@ -426,7 +430,7 @@
                   <c:v>Aufgabenstellung erfassen</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Mockups erstellen</c:v>
+                  <c:v>Anforderungen definieren</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Zwischenpräsentation planen</c:v>
@@ -438,48 +442,51 @@
                   <c:v>M1: Abschluss Projektplan</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Anforderungen definieren</c:v>
+                  <c:v>Mockups erstellen</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Detailkonzept</c:v>
+                  <c:v>Datenbankschema planen</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>Sequenzdiagramme erstellt</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Architektur planen</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Domainanalyse</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>M2: End of Elaboration</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Infrastruktur einrichten</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Backend entwickeln</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>UI entwickeln</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Testing</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>M3: Feature Freeze</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Bugfixes</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>M4: Code Freeze</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>Dokumentation</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>Präsentation</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>M5: Projektende</c:v>
                 </c:pt>
               </c:strCache>
@@ -487,10 +494,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Projektplan!$E$9:$E$33</c:f>
+              <c:f>Projektplan!$E$9:$E$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -513,19 +520,19 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>22</c:v>
@@ -534,24 +541,27 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>63</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>77</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>78</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>91</c:v>
                 </c:pt>
               </c:numCache>
@@ -643,9 +653,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Projektplan!$B$9:$B$33</c:f>
+              <c:f>Projektplan!$B$9:$B$34</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>M0: Kickoff</c:v>
                 </c:pt>
@@ -653,7 +663,7 @@
                   <c:v>Aufgabenstellung erfassen</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Mockups erstellen</c:v>
+                  <c:v>Anforderungen definieren</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Zwischenpräsentation planen</c:v>
@@ -665,48 +675,51 @@
                   <c:v>M1: Abschluss Projektplan</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Anforderungen definieren</c:v>
+                  <c:v>Mockups erstellen</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Detailkonzept</c:v>
+                  <c:v>Datenbankschema planen</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>Sequenzdiagramme erstellt</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Architektur planen</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Domainanalyse</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>M2: End of Elaboration</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Infrastruktur einrichten</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Backend entwickeln</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>UI entwickeln</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Testing</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>M3: Feature Freeze</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Bugfixes</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>M4: Code Freeze</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>Dokumentation</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>Präsentation</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>M5: Projektende</c:v>
                 </c:pt>
               </c:strCache>
@@ -714,10 +727,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Projektplan!$F$9:$F$33</c:f>
+              <c:f>Projektplan!$F$9:$F$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -725,7 +738,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
@@ -737,48 +750,51 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -881,7 +897,7 @@
             <a:pPr lvl="0">
               <a:defRPr b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1334299962"/>
@@ -1239,24 +1255,24 @@
   </sheetPr>
   <dimension ref="A1:AL50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="91" zoomScaleNormal="213" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="91" zoomScaleNormal="213" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="10" width="7.28515625" customWidth="1"/>
-    <col min="11" max="12" width="3.7109375" customWidth="1"/>
-    <col min="13" max="13" width="6.42578125" customWidth="1"/>
-    <col min="14" max="32" width="4.42578125" customWidth="1"/>
-    <col min="33" max="33" width="7.28515625" customWidth="1"/>
-    <col min="34" max="34" width="7.140625" customWidth="1"/>
-    <col min="36" max="37" width="0.140625" customWidth="1"/>
-    <col min="38" max="38" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" customWidth="1"/>
+    <col min="3" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="10" width="7.33203125" customWidth="1"/>
+    <col min="11" max="12" width="3.6640625" customWidth="1"/>
+    <col min="13" max="13" width="6.5" customWidth="1"/>
+    <col min="14" max="32" width="4.5" customWidth="1"/>
+    <col min="33" max="33" width="7.33203125" customWidth="1"/>
+    <col min="34" max="34" width="7.1640625" customWidth="1"/>
+    <col min="36" max="37" width="0.1640625" customWidth="1"/>
+    <col min="38" max="38" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="15.75" customHeight="1">
@@ -1332,16 +1348,16 @@
       <c r="AH2" s="2"/>
     </row>
     <row r="3" spans="1:38" ht="30" customHeight="1">
-      <c r="A3" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+      <c r="A3" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="3"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -1443,64 +1459,64 @@
       <c r="AH5" s="2"/>
     </row>
     <row r="6" spans="1:38" ht="15">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="31"/>
-      <c r="V6" s="31"/>
-      <c r="W6" s="31"/>
-      <c r="X6" s="30"/>
-      <c r="Y6" s="31"/>
-      <c r="Z6" s="31"/>
-      <c r="AA6" s="31"/>
-      <c r="AB6" s="31"/>
-      <c r="AC6" s="30"/>
-      <c r="AD6" s="31"/>
-      <c r="AE6" s="31"/>
-      <c r="AF6" s="31"/>
-      <c r="AG6" s="31"/>
-      <c r="AH6" s="30"/>
-      <c r="AI6" s="31"/>
-      <c r="AJ6" s="31"/>
-      <c r="AK6" s="31"/>
-      <c r="AL6" s="31"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="35"/>
+      <c r="Y6" s="36"/>
+      <c r="Z6" s="36"/>
+      <c r="AA6" s="36"/>
+      <c r="AB6" s="36"/>
+      <c r="AC6" s="35"/>
+      <c r="AD6" s="36"/>
+      <c r="AE6" s="36"/>
+      <c r="AF6" s="36"/>
+      <c r="AG6" s="36"/>
+      <c r="AH6" s="35"/>
+      <c r="AI6" s="36"/>
+      <c r="AJ6" s="36"/>
+      <c r="AK6" s="36"/>
+      <c r="AL6" s="36"/>
     </row>
     <row r="7" spans="1:38" ht="15">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
@@ -1528,9 +1544,9 @@
       <c r="AG7" s="9"/>
       <c r="AH7" s="9"/>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" ht="16">
       <c r="A8" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1565,9 +1581,9 @@
       <c r="AG8" s="12"/>
       <c r="AH8" s="12"/>
     </row>
-    <row r="9" spans="1:38" ht="15">
+    <row r="9" spans="1:38" ht="16">
       <c r="B9" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="25">
         <v>43749</v>
@@ -1613,9 +1629,9 @@
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
     </row>
-    <row r="10" spans="1:38" ht="15">
+    <row r="10" spans="1:38" ht="16">
       <c r="B10" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="25">
         <v>43750</v>
@@ -1628,7 +1644,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="23">
-        <f t="shared" ref="F10:F32" si="1">DATEDIF(C10,D10,"d")+1</f>
+        <f t="shared" ref="F10:F33" si="1">DATEDIF(C10,D10,"d")+1</f>
         <v>2</v>
       </c>
       <c r="G10" s="18">
@@ -1661,16 +1677,16 @@
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
     </row>
-    <row r="11" spans="1:38" ht="15">
+    <row r="11" spans="1:38" ht="16">
       <c r="A11" s="24"/>
       <c r="B11" s="15" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C11" s="25">
         <v>43750</v>
       </c>
       <c r="D11" s="27">
-        <v>43750</v>
+        <v>43753</v>
       </c>
       <c r="E11" s="16">
         <f>INT(C11)-INT($C$9)</f>
@@ -1678,7 +1694,7 @@
       </c>
       <c r="F11" s="23">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G11" s="18">
         <v>1</v>
@@ -1710,10 +1726,10 @@
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
     </row>
-    <row r="12" spans="1:38" ht="15">
+    <row r="12" spans="1:38" ht="16">
       <c r="A12" s="24"/>
       <c r="B12" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="25">
         <v>43754</v>
@@ -1730,13 +1746,13 @@
         <v>2</v>
       </c>
       <c r="G12" s="18">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:38" ht="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" ht="16">
       <c r="A13" s="24"/>
       <c r="B13" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="25">
         <v>43751</v>
@@ -1753,12 +1769,12 @@
         <v>5</v>
       </c>
       <c r="G13" s="18">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:38" ht="15">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" ht="16">
       <c r="B14" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="25">
         <v>43756</v>
@@ -1775,12 +1791,12 @@
         <v>1</v>
       </c>
       <c r="G14" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" ht="16">
       <c r="A15" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="26"/>
@@ -1789,175 +1805,176 @@
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="1:38" ht="15">
+    <row r="16" spans="1:38" ht="16">
       <c r="B16" s="15" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C16" s="25">
         <v>43757</v>
       </c>
       <c r="D16" s="27">
-        <v>43760</v>
+        <v>43763</v>
       </c>
       <c r="E16" s="16">
-        <f t="shared" ref="E16:E20" si="2">INT(C16)-INT($C$9)</f>
+        <f t="shared" ref="E16:E21" si="2">INT(C16)-INT($C$9)</f>
         <v>8</v>
       </c>
       <c r="F16" s="23">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G16" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16">
+      <c r="A17" s="30"/>
       <c r="B17" s="15" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C17" s="25">
-        <v>43760</v>
+        <v>43757</v>
       </c>
       <c r="D17" s="27">
-        <v>43761</v>
+        <v>43765</v>
       </c>
       <c r="E17" s="16">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F17" s="23">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G17" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15">
-      <c r="A18" s="24"/>
+        <v>9</v>
+      </c>
+      <c r="G17" s="20">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16">
       <c r="B18" s="15" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C18" s="25">
-        <v>43763</v>
+        <v>43766</v>
       </c>
       <c r="D18" s="27">
-        <v>43765</v>
+        <v>43770</v>
       </c>
       <c r="E18" s="16">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F18" s="23">
-        <f t="shared" ref="F18" si="3">DATEDIF(C18,D18,"d")+1</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="G18" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15">
+    <row r="19" spans="1:7" ht="16">
+      <c r="A19" s="24"/>
       <c r="B19" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" s="25">
-        <v>43766</v>
+        <v>43767</v>
       </c>
       <c r="D19" s="27">
-        <v>43769</v>
+        <v>43770</v>
       </c>
       <c r="E19" s="16">
         <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="F19" s="23">
+        <f t="shared" ref="F19" si="3">DATEDIF(C19,D19,"d")+1</f>
+        <v>4</v>
+      </c>
+      <c r="G19" s="21">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16">
+      <c r="B20" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="25">
+        <v>43766</v>
+      </c>
+      <c r="D20" s="27">
+        <v>43769</v>
+      </c>
+      <c r="E20" s="16">
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F20" s="23">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G20" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15">
-      <c r="B20" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="25">
+    <row r="21" spans="1:7" ht="16">
+      <c r="B21" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="25">
         <v>43770</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D21" s="27">
         <v>43770</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E21" s="16">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F21" s="23">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G21" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-    </row>
-    <row r="22" spans="1:7" ht="15">
-      <c r="B22" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="25">
+    <row r="22" spans="1:7" ht="16">
+      <c r="A22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+    </row>
+    <row r="23" spans="1:7" ht="16">
+      <c r="B23" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="25">
         <v>43771</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D23" s="27">
         <v>43771</v>
       </c>
-      <c r="E22" s="16">
-        <f t="shared" ref="E22:E28" si="4">INT(C22)-INT($C$9)</f>
+      <c r="E23" s="16">
+        <f t="shared" ref="E23:E29" si="4">INT(C23)-INT($C$9)</f>
         <v>22</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F23" s="23">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G22" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15">
-      <c r="B23" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="25">
-        <v>43771</v>
-      </c>
-      <c r="D23" s="27">
-        <v>43811</v>
-      </c>
-      <c r="E23" s="16">
-        <f t="shared" si="4"/>
-        <v>22</v>
-      </c>
-      <c r="F23" s="23">
-        <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
       <c r="G23" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15">
-      <c r="B24" s="29" t="s">
-        <v>10</v>
+    <row r="24" spans="1:7" ht="16">
+      <c r="B24" s="15" t="s">
+        <v>8</v>
       </c>
       <c r="C24" s="25">
         <v>43771</v>
@@ -1977,190 +1994,203 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15">
-      <c r="B25" s="15" t="s">
-        <v>11</v>
+    <row r="25" spans="1:7" ht="16">
+      <c r="B25" s="29" t="s">
+        <v>9</v>
       </c>
       <c r="C25" s="25">
-        <v>43800</v>
+        <v>43771</v>
       </c>
       <c r="D25" s="27">
         <v>43811</v>
       </c>
       <c r="E25" s="16">
         <f t="shared" si="4"/>
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="F25" s="23">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="G25" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15">
-      <c r="B26" s="28" t="s">
-        <v>27</v>
+    <row r="26" spans="1:7" ht="16">
+      <c r="B26" s="15" t="s">
+        <v>10</v>
       </c>
       <c r="C26" s="25">
-        <v>43812</v>
+        <v>43800</v>
       </c>
       <c r="D26" s="27">
-        <v>43812</v>
+        <v>43811</v>
       </c>
       <c r="E26" s="16">
         <f t="shared" si="4"/>
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F26" s="23">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G26" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15">
-      <c r="A27" s="24"/>
-      <c r="B27" s="15" t="s">
-        <v>32</v>
+    <row r="27" spans="1:7" ht="16">
+      <c r="B27" s="28" t="s">
+        <v>26</v>
       </c>
       <c r="C27" s="25">
-        <v>43813</v>
+        <v>43812</v>
       </c>
       <c r="D27" s="27">
-        <v>43826</v>
+        <v>43812</v>
       </c>
       <c r="E27" s="16">
         <f t="shared" si="4"/>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F27" s="23">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G27" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15">
+    <row r="28" spans="1:7" ht="16">
       <c r="A28" s="24"/>
-      <c r="B28" s="28" t="s">
-        <v>28</v>
+      <c r="B28" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="C28" s="25">
-        <v>43826</v>
+        <v>43813</v>
       </c>
       <c r="D28" s="27">
         <v>43826</v>
       </c>
       <c r="E28" s="16">
         <f t="shared" si="4"/>
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F28" s="23">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G28" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
+    <row r="29" spans="1:7" ht="16">
+      <c r="A29" s="24"/>
+      <c r="B29" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="25">
+        <v>43826</v>
+      </c>
+      <c r="D29" s="27">
+        <v>43826</v>
+      </c>
+      <c r="E29" s="16">
+        <f t="shared" si="4"/>
+        <v>77</v>
+      </c>
+      <c r="F29" s="23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G29" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B30" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="25">
+      <c r="A30" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="19"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B31" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="25">
         <v>43827</v>
       </c>
-      <c r="D30" s="27">
+      <c r="D31" s="27">
         <v>43840</v>
       </c>
-      <c r="E30" s="16">
-        <f t="shared" ref="E30:E32" si="5">INT(C30)-INT($C$9)</f>
+      <c r="E31" s="16">
+        <f t="shared" ref="E31:E33" si="5">INT(C31)-INT($C$9)</f>
         <v>78</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F31" s="23">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="G30" s="22">
+      <c r="G31" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B31" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="25">
+    <row r="32" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B32" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="25">
         <v>43837</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D32" s="27">
         <v>43840</v>
       </c>
-      <c r="E31" s="16">
+      <c r="E32" s="16">
         <f t="shared" si="5"/>
         <v>88</v>
       </c>
-      <c r="F31" s="23">
+      <c r="F32" s="23">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G32" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B32" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="25">
+    <row r="33" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B33" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="25">
         <v>43840</v>
       </c>
-      <c r="D32" s="27">
+      <c r="D33" s="27">
         <v>43840</v>
       </c>
-      <c r="E32" s="16">
+      <c r="E33" s="16">
         <f t="shared" si="5"/>
         <v>91</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F33" s="23">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G32" s="22">
+      <c r="G33" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B33" s="28"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="29"/>
       <c r="H33" s="22"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="29"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1">
@@ -2173,7 +2203,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="12.75">
+    <row r="36" spans="1:8" ht="13">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2183,22 +2213,36 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="12.75"/>
-    <row r="38" spans="1:8" ht="12.75"/>
-    <row r="39" spans="1:8" ht="12.75"/>
-    <row r="40" spans="1:8" ht="12.75"/>
-    <row r="41" spans="1:8" ht="12.75"/>
-    <row r="42" spans="1:8" ht="12.75"/>
-    <row r="43" spans="1:8" ht="12.75"/>
-    <row r="44" spans="1:8" ht="12.75"/>
-    <row r="45" spans="1:8" ht="12.75"/>
-    <row r="46" spans="1:8" ht="12.75"/>
-    <row r="47" spans="1:8" ht="12.75"/>
-    <row r="48" spans="1:8" ht="12.75"/>
-    <row r="49" ht="12.75"/>
-    <row r="50" ht="12.75"/>
+    <row r="37" spans="1:8" ht="13">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" ht="13"/>
+    <row r="39" spans="1:8" ht="13"/>
+    <row r="40" spans="1:8" ht="13"/>
+    <row r="41" spans="1:8" ht="13"/>
+    <row r="42" spans="1:8" ht="13"/>
+    <row r="43" spans="1:8" ht="13"/>
+    <row r="44" spans="1:8" ht="13"/>
+    <row r="45" spans="1:8" ht="13"/>
+    <row r="46" spans="1:8" ht="13"/>
+    <row r="47" spans="1:8" ht="13"/>
+    <row r="48" spans="1:8" ht="13"/>
+    <row r="49" ht="13"/>
+    <row r="50" ht="13"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AH6:AL6"/>
+    <mergeCell ref="AC6:AG6"/>
+    <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="S6:W6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="N6:R6"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="E6:E7"/>
@@ -2207,14 +2251,8 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="AH6:AL6"/>
-    <mergeCell ref="AC6:AG6"/>
-    <mergeCell ref="X6:AB6"/>
-    <mergeCell ref="S6:W6"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="N6:R6"/>
   </mergeCells>
-  <conditionalFormatting sqref="G30:G32 H33 G9:G14 G22:G28 G16:G20">
+  <conditionalFormatting sqref="G31:G33 H33 G9:G14 G23:G29 G16:G21">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percent" val="0"/>
@@ -2225,7 +2263,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C30:D33 C9:D14 D16:D20 D22:D28" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C31:D34 C9:D14 D23:D29 D16:D21" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>OR(NOT(ISERROR(DATEVALUE(C9))), AND(ISNUMBER(C9), LEFT(CELL("format", C9))="D"))</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Improve project plan according to feedback provided by Frank Koch
</commit_message>
<xml_diff>
--- a/Projektplan.xlsx
+++ b/Projektplan.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HSR\BA\BA-Projektplan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\HSR\Module\_BA\Dokumente\BA-Projektplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D38D74-031B-4DAB-B1F7-23DEABFF2824}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2746933E-A205-486C-B687-6D946AEA5A0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplan" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>TASK NAME</t>
   </si>
@@ -43,21 +51,9 @@
     <t>DURATION* (WORK DAYS)</t>
   </si>
   <si>
-    <t>Infrastruktur einrichten</t>
-  </si>
-  <si>
-    <t>Backend entwickeln</t>
-  </si>
-  <si>
-    <t>UI entwickeln</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
-    <t>Projekt ToDo Verwaltung</t>
-  </si>
-  <si>
     <t>Inception</t>
   </si>
   <si>
@@ -131,6 +127,36 @@
   </si>
   <si>
     <t>Abgabe vorbereiten</t>
+  </si>
+  <si>
+    <t>UC CRUD class</t>
+  </si>
+  <si>
+    <t>UC CRUD person</t>
+  </si>
+  <si>
+    <t>UC CRUD task</t>
+  </si>
+  <si>
+    <t>UC CRUD quiz</t>
+  </si>
+  <si>
+    <t>UC publish study content</t>
+  </si>
+  <si>
+    <t>UC solve task</t>
+  </si>
+  <si>
+    <t>UC solve quiz</t>
+  </si>
+  <si>
+    <t>UC view statistics</t>
+  </si>
+  <si>
+    <t>UC send message</t>
+  </si>
+  <si>
+    <t>Projekt Aufgaben Coach Verwaltung</t>
   </si>
 </sst>
 </file>
@@ -140,7 +166,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -214,12 +240,6 @@
     <font>
       <sz val="26"/>
       <color rgb="FF576C88"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF434343"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -301,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -365,27 +385,29 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF5CBCD6"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -400,7 +422,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -422,9 +444,9 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>Projektplan!$B$9:$B$36</c:f>
+              <c:f>Projektplan!$B$9:$B$42</c:f>
               <c:strCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>M0: Kickoff</c:v>
                 </c:pt>
@@ -435,10 +457,10 @@
                   <c:v>Anforderungen definieren</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Projektplan erstellen</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Zwischenpräsentation planen</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Projektplan erstellen</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>M1: Abschluss Projektplan</c:v>
@@ -456,48 +478,66 @@
                   <c:v>Use Cases ausarbeiten</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Domainanalyse</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Sequenzdiagramme erstellen</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Architektur planen</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Domainanalyse</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>M2: End of Elaboration</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Infrastruktur einrichten</c:v>
+                  <c:v>UC CRUD class</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Backend entwickeln</c:v>
+                  <c:v>UC CRUD person</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>UI entwickeln</c:v>
+                  <c:v>UC CRUD task</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>UC CRUD quiz</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>UC publish study content</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>UC solve task</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>UC solve quiz</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>UC view statistics</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>UC send message</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>M3: Feature Freeze</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Bugfixes</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>Testing</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>M3: Feature Freeze</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Bugfixes</c:v>
-                </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="28">
                   <c:v>M4: Code Freeze</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="30">
                   <c:v>Dokumentation abschliessen</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="31">
                   <c:v>Abgabe vorbereiten</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="32">
                   <c:v>M5: Projektende</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="33">
                   <c:v>Präsentation vorbereiten</c:v>
                 </c:pt>
               </c:strCache>
@@ -505,10 +545,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Projektplan!$E$9:$E$36</c:f>
+              <c:f>Projektplan!$E$9:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -519,10 +559,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>7</c:v>
@@ -543,10 +583,10 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>21</c:v>
@@ -561,28 +601,46 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="27">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>77</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="30">
                   <c:v>78</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="31">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="32">
                   <c:v>91</c:v>
                 </c:pt>
-                <c:pt idx="27">
-                  <c:v>91</c:v>
+                <c:pt idx="33">
+                  <c:v>92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -612,7 +670,7 @@
           </c:spPr>
           <c:invertIfNegative val="1"/>
           <c:dPt>
-            <c:idx val="2"/>
+            <c:idx val="0"/>
             <c:invertIfNegative val="1"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -622,7 +680,37 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-A02A-4E6F-8D20-96E275048E84}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="5CBCD6"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000000-CA47-6B4E-A35A-2383EBA7A049}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-A02A-4E6F-8D20-96E275048E84}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -632,7 +720,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="5CBCD6"/>
               </a:solidFill>
             </c:spPr>
             <c:extLst>
@@ -647,7 +735,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="5CBCD6"/>
               </a:solidFill>
             </c:spPr>
             <c:extLst>
@@ -657,7 +745,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="18"/>
+            <c:idx val="14"/>
             <c:invertIfNegative val="1"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -667,15 +755,75 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-A02A-4E6F-8D20-96E275048E84}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="5CBCD6"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-CA47-6B4E-A35A-2383EBA7A049}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="25"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-A02A-4E6F-8D20-96E275048E84}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="28"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-A02A-4E6F-8D20-96E275048E84}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="32"/>
+            <c:invertIfNegative val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-A02A-4E6F-8D20-96E275048E84}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Projektplan!$B$9:$B$36</c:f>
+              <c:f>Projektplan!$B$9:$B$42</c:f>
               <c:strCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>M0: Kickoff</c:v>
                 </c:pt>
@@ -686,10 +834,10 @@
                   <c:v>Anforderungen definieren</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Projektplan erstellen</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Zwischenpräsentation planen</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Projektplan erstellen</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>M1: Abschluss Projektplan</c:v>
@@ -707,48 +855,66 @@
                   <c:v>Use Cases ausarbeiten</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Domainanalyse</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Sequenzdiagramme erstellen</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Architektur planen</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Domainanalyse</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>M2: End of Elaboration</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Infrastruktur einrichten</c:v>
+                  <c:v>UC CRUD class</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Backend entwickeln</c:v>
+                  <c:v>UC CRUD person</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>UI entwickeln</c:v>
+                  <c:v>UC CRUD task</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>UC CRUD quiz</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>UC publish study content</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>UC solve task</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>UC solve quiz</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>UC view statistics</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>UC send message</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>M3: Feature Freeze</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Bugfixes</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>Testing</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>M3: Feature Freeze</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Bugfixes</c:v>
-                </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="28">
                   <c:v>M4: Code Freeze</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="30">
                   <c:v>Dokumentation abschliessen</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="31">
                   <c:v>Abgabe vorbereiten</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="32">
                   <c:v>M5: Projektende</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="33">
                   <c:v>Präsentation vorbereiten</c:v>
                 </c:pt>
               </c:strCache>
@@ -756,10 +922,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Projektplan!$F$9:$F$36</c:f>
+              <c:f>Projektplan!$F$9:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -770,10 +936,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -791,10 +957,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>4</c:v>
@@ -803,37 +969,55 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="26">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="30">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="31">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>21</c:v>
+                <c:pt idx="33">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -960,11 +1144,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>191895</xdr:colOff>
+      <xdr:colOff>191894</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>94204</xdr:rowOff>
+      <xdr:rowOff>94203</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="10006483" cy="4633406"/>
+    <xdr:ext cx="10515879" cy="7012912"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1" title="Chart">
@@ -992,7 +1176,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1293,11 +1477,11 @@
   </sheetPr>
   <dimension ref="A1:AL50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="91" zoomScaleNormal="213" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" customWidth="1"/>
@@ -1386,16 +1570,16 @@
       <c r="AH2" s="2"/>
     </row>
     <row r="3" spans="1:38" ht="30" customHeight="1">
-      <c r="A3" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="A3" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="3"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -1497,64 +1681,64 @@
       <c r="AH5" s="2"/>
     </row>
     <row r="6" spans="1:38" ht="15">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="32"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="33"/>
-      <c r="V6" s="33"/>
-      <c r="W6" s="33"/>
-      <c r="X6" s="32"/>
-      <c r="Y6" s="33"/>
-      <c r="Z6" s="33"/>
-      <c r="AA6" s="33"/>
-      <c r="AB6" s="33"/>
-      <c r="AC6" s="32"/>
-      <c r="AD6" s="33"/>
-      <c r="AE6" s="33"/>
-      <c r="AF6" s="33"/>
-      <c r="AG6" s="33"/>
-      <c r="AH6" s="32"/>
-      <c r="AI6" s="33"/>
-      <c r="AJ6" s="33"/>
-      <c r="AK6" s="33"/>
-      <c r="AL6" s="33"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="35"/>
+      <c r="Y6" s="36"/>
+      <c r="Z6" s="36"/>
+      <c r="AA6" s="36"/>
+      <c r="AB6" s="36"/>
+      <c r="AC6" s="35"/>
+      <c r="AD6" s="36"/>
+      <c r="AE6" s="36"/>
+      <c r="AF6" s="36"/>
+      <c r="AG6" s="36"/>
+      <c r="AH6" s="35"/>
+      <c r="AI6" s="36"/>
+      <c r="AJ6" s="36"/>
+      <c r="AK6" s="36"/>
+      <c r="AL6" s="36"/>
     </row>
     <row r="7" spans="1:38" ht="15">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
@@ -1584,7 +1768,7 @@
     </row>
     <row r="8" spans="1:38">
       <c r="A8" s="11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1621,7 +1805,7 @@
     </row>
     <row r="9" spans="1:38" ht="15">
       <c r="B9" s="28" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C9" s="25">
         <v>43749</v>
@@ -1669,7 +1853,7 @@
     </row>
     <row r="10" spans="1:38" ht="15">
       <c r="B10" s="15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C10" s="25">
         <v>43750</v>
@@ -1682,7 +1866,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="23">
-        <f t="shared" ref="F10:F36" si="1">DATEDIF(C10,D10,"d")+1</f>
+        <f t="shared" ref="F10:F34" si="1">DATEDIF(C10,D10,"d")+1</f>
         <v>2</v>
       </c>
       <c r="G10" s="18">
@@ -1718,7 +1902,7 @@
     <row r="11" spans="1:38" ht="15">
       <c r="A11" s="24"/>
       <c r="B11" s="15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" s="25">
         <v>43750</v>
@@ -1767,21 +1951,21 @@
     <row r="12" spans="1:38" ht="15">
       <c r="A12" s="24"/>
       <c r="B12" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="25">
-        <v>43754</v>
+        <v>43751</v>
       </c>
       <c r="D12" s="27">
         <v>43755</v>
       </c>
       <c r="E12" s="16">
         <f>INT(C12)-INT($C$9)</f>
+        <v>2</v>
+      </c>
+      <c r="F12" s="23">
+        <f>DATEDIF(C12,D12,"d")+1</f>
         <v>5</v>
-      </c>
-      <c r="F12" s="23">
-        <f t="shared" si="1"/>
-        <v>2</v>
       </c>
       <c r="G12" s="18">
         <v>1</v>
@@ -1790,21 +1974,21 @@
     <row r="13" spans="1:38" ht="15">
       <c r="A13" s="24"/>
       <c r="B13" s="15" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C13" s="25">
-        <v>43751</v>
+        <v>43754</v>
       </c>
       <c r="D13" s="27">
         <v>43755</v>
       </c>
       <c r="E13" s="16">
         <f>INT(C13)-INT($C$9)</f>
+        <v>5</v>
+      </c>
+      <c r="F13" s="23">
+        <f t="shared" ref="F13" si="2">DATEDIF(C13,D13,"d")+1</f>
         <v>2</v>
-      </c>
-      <c r="F13" s="23">
-        <f>DATEDIF(C13,D13,"d")+1</f>
-        <v>5</v>
       </c>
       <c r="G13" s="18">
         <v>1</v>
@@ -1812,7 +1996,7 @@
     </row>
     <row r="14" spans="1:38" ht="15">
       <c r="B14" s="28" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C14" s="25">
         <v>43756</v>
@@ -1834,7 +2018,7 @@
     </row>
     <row r="15" spans="1:38">
       <c r="A15" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="26"/>
@@ -1845,7 +2029,7 @@
     </row>
     <row r="16" spans="1:38" ht="15">
       <c r="B16" s="15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C16" s="25">
         <v>43757</v>
@@ -1854,7 +2038,7 @@
         <v>43763</v>
       </c>
       <c r="E16" s="16">
-        <f t="shared" ref="E16:E23" si="2">INT(C16)-INT($C$9)</f>
+        <f t="shared" ref="E16:E23" si="3">INT(C16)-INT($C$9)</f>
         <v>8</v>
       </c>
       <c r="F16" s="23">
@@ -1862,13 +2046,13 @@
         <v>7</v>
       </c>
       <c r="G16" s="20">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15">
-      <c r="A17" s="30"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" s="25">
         <v>43757</v>
@@ -1877,7 +2061,7 @@
         <v>43763</v>
       </c>
       <c r="E17" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="F17" s="23">
@@ -1885,13 +2069,13 @@
         <v>7</v>
       </c>
       <c r="G17" s="20">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A18" s="31"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C18" s="25">
         <v>43761</v>
@@ -1900,7 +2084,7 @@
         <v>43761</v>
       </c>
       <c r="E18" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="F18" s="23">
@@ -1912,9 +2096,9 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15">
-      <c r="A19" s="31"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C19" s="25">
         <v>43762</v>
@@ -1923,7 +2107,7 @@
         <v>43765</v>
       </c>
       <c r="E19" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="F19" s="23">
@@ -1931,26 +2115,26 @@
         <v>4</v>
       </c>
       <c r="G19" s="20">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="15" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C20" s="25">
         <v>43766</v>
       </c>
       <c r="D20" s="27">
-        <v>43770</v>
+        <v>43769</v>
       </c>
       <c r="E20" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E20" si="4">INT(C20)-INT($C$9)</f>
         <v>17</v>
       </c>
       <c r="F20" s="23">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f t="shared" ref="F20" si="5">DATEDIF(C20,D20,"d")+1</f>
+        <v>4</v>
       </c>
       <c r="G20" s="21">
         <v>0</v>
@@ -1959,21 +2143,21 @@
     <row r="21" spans="1:7" ht="15">
       <c r="A21" s="24"/>
       <c r="B21" s="15" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C21" s="25">
-        <v>43767</v>
+        <v>43766</v>
       </c>
       <c r="D21" s="27">
         <v>43770</v>
       </c>
       <c r="E21" s="16">
-        <f t="shared" si="2"/>
-        <v>18</v>
+        <f>INT(C21)-INT($C$9)</f>
+        <v>17</v>
       </c>
       <c r="F21" s="23">
-        <f t="shared" ref="F21" si="3">DATEDIF(C21,D21,"d")+1</f>
-        <v>4</v>
+        <f>DATEDIF(C21,D21,"d")+1</f>
+        <v>5</v>
       </c>
       <c r="G21" s="21">
         <v>0.2</v>
@@ -1981,20 +2165,20 @@
     </row>
     <row r="22" spans="1:7" ht="15">
       <c r="B22" s="15" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C22" s="25">
-        <v>43766</v>
+        <v>43767</v>
       </c>
       <c r="D22" s="27">
-        <v>43769</v>
+        <v>43770</v>
       </c>
       <c r="E22" s="16">
-        <f t="shared" si="2"/>
-        <v>17</v>
+        <f>INT(C22)-INT($C$9)</f>
+        <v>18</v>
       </c>
       <c r="F22" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F22" si="6">DATEDIF(C22,D22,"d")+1</f>
         <v>4</v>
       </c>
       <c r="G22" s="22">
@@ -2003,7 +2187,7 @@
     </row>
     <row r="23" spans="1:7" ht="15">
       <c r="B23" s="28" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C23" s="25">
         <v>43770</v>
@@ -2012,7 +2196,7 @@
         <v>43770</v>
       </c>
       <c r="E23" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="F23" s="23">
@@ -2025,7 +2209,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="26"/>
@@ -2036,21 +2220,21 @@
     </row>
     <row r="25" spans="1:7" ht="15">
       <c r="B25" s="15" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C25" s="25">
         <v>43771</v>
       </c>
       <c r="D25" s="27">
-        <v>43771</v>
+        <v>43785</v>
       </c>
       <c r="E25" s="16">
-        <f t="shared" ref="E25:E31" si="4">INT(C25)-INT($C$9)</f>
+        <f t="shared" ref="E25:E31" si="7">INT(C25)-INT($C$9)</f>
         <v>22</v>
       </c>
       <c r="F25" s="23">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G25" s="22">
         <v>0</v>
@@ -2058,43 +2242,43 @@
     </row>
     <row r="26" spans="1:7" ht="15">
       <c r="B26" s="15" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C26" s="25">
         <v>43771</v>
       </c>
       <c r="D26" s="27">
-        <v>43811</v>
+        <v>43785</v>
       </c>
       <c r="E26" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
       <c r="F26" s="23">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="G26" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15">
-      <c r="B27" s="29" t="s">
-        <v>9</v>
+      <c r="B27" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="C27" s="25">
         <v>43771</v>
       </c>
       <c r="D27" s="27">
-        <v>43811</v>
+        <v>43785</v>
       </c>
       <c r="E27" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
       <c r="F27" s="23">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="G27" s="22">
         <v>0</v>
@@ -2102,122 +2286,131 @@
     </row>
     <row r="28" spans="1:7" ht="15">
       <c r="B28" s="15" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C28" s="25">
-        <v>43800</v>
+        <v>43771</v>
       </c>
       <c r="D28" s="27">
-        <v>43811</v>
+        <v>43785</v>
       </c>
       <c r="E28" s="16">
-        <f t="shared" si="4"/>
-        <v>51</v>
+        <f t="shared" ref="E28:E32" si="8">INT(C28)-INT($C$9)</f>
+        <v>22</v>
       </c>
       <c r="F28" s="23">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" ref="F28:F32" si="9">DATEDIF(C28,D28,"d")+1</f>
+        <v>15</v>
       </c>
       <c r="G28" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15">
-      <c r="B29" s="28" t="s">
-        <v>26</v>
+      <c r="B29" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="C29" s="25">
-        <v>43812</v>
+        <v>43785</v>
       </c>
       <c r="D29" s="27">
-        <v>43812</v>
+        <v>43799</v>
       </c>
       <c r="E29" s="16">
-        <f t="shared" si="4"/>
-        <v>63</v>
+        <f t="shared" si="8"/>
+        <v>36</v>
       </c>
       <c r="F29" s="23">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="9"/>
+        <v>15</v>
       </c>
       <c r="G29" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A30" s="24"/>
       <c r="B30" s="15" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C30" s="25">
-        <v>43813</v>
+        <v>43785</v>
       </c>
       <c r="D30" s="27">
-        <v>43826</v>
+        <v>43799</v>
       </c>
       <c r="E30" s="16">
-        <f t="shared" si="4"/>
-        <v>64</v>
+        <f t="shared" si="8"/>
+        <v>36</v>
       </c>
       <c r="F30" s="23">
-        <f t="shared" si="1"/>
-        <v>14</v>
+        <f t="shared" si="9"/>
+        <v>15</v>
       </c>
       <c r="G30" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A31" s="24"/>
-      <c r="B31" s="28" t="s">
-        <v>27</v>
+      <c r="B31" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="C31" s="25">
-        <v>43826</v>
+        <v>43785</v>
       </c>
       <c r="D31" s="27">
-        <v>43826</v>
+        <v>43799</v>
       </c>
       <c r="E31" s="16">
-        <f t="shared" si="4"/>
-        <v>77</v>
+        <f t="shared" si="8"/>
+        <v>36</v>
       </c>
       <c r="F31" s="23">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="9"/>
+        <v>15</v>
       </c>
       <c r="G31" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A32" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
+      <c r="B32" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="25">
+        <v>43800</v>
+      </c>
+      <c r="D32" s="27">
+        <v>43811</v>
+      </c>
+      <c r="E32" s="16">
+        <f t="shared" si="8"/>
+        <v>51</v>
+      </c>
+      <c r="F32" s="23">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="G32" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1">
       <c r="B33" s="15" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C33" s="25">
-        <v>43827</v>
+        <v>43800</v>
       </c>
       <c r="D33" s="27">
-        <v>43840</v>
+        <v>43811</v>
       </c>
       <c r="E33" s="16">
-        <f t="shared" ref="E33:E36" si="5">INT(C33)-INT($C$9)</f>
-        <v>78</v>
+        <f>INT(C33)-INT($C$9)</f>
+        <v>51</v>
       </c>
       <c r="F33" s="23">
-        <f t="shared" si="1"/>
-        <v>14</v>
+        <f>DATEDIF(C33,D33,"d")+1</f>
+        <v>12</v>
       </c>
       <c r="G33" s="22">
         <v>0</v>
@@ -2225,23 +2418,22 @@
       <c r="H33" s="22"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A34" s="31"/>
       <c r="B34" s="15" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C34" s="25">
-        <v>43839</v>
+        <v>43811</v>
       </c>
       <c r="D34" s="27">
-        <v>43840</v>
+        <v>43811</v>
       </c>
       <c r="E34" s="16">
-        <f t="shared" si="5"/>
-        <v>90</v>
+        <f>INT(C34)-INT($C$9)</f>
+        <v>62</v>
       </c>
       <c r="F34" s="23">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f>DATEDIF(C34,D34,"d")+1</f>
+        <v>1</v>
       </c>
       <c r="G34" s="22">
         <v>0</v>
@@ -2249,22 +2441,23 @@
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B35" s="28" t="s">
-        <v>28</v>
+      <c r="A35" s="24"/>
+      <c r="B35" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="C35" s="25">
-        <v>43840</v>
+        <v>43813</v>
       </c>
       <c r="D35" s="27">
-        <v>43840</v>
+        <v>43826</v>
       </c>
       <c r="E35" s="16">
         <f>INT(C35)-INT($C$9)</f>
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="F35" s="23">
         <f>DATEDIF(C35,D35,"d")+1</f>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G35" s="22">
         <v>0</v>
@@ -2273,60 +2466,149 @@
     </row>
     <row r="36" spans="1:8" ht="15">
       <c r="B36" s="15" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C36" s="25">
-        <v>43840</v>
+        <v>43813</v>
       </c>
       <c r="D36" s="27">
-        <v>43860</v>
+        <v>43826</v>
       </c>
       <c r="E36" s="16">
         <f>INT(C36)-INT($C$9)</f>
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="F36" s="23">
         <f>DATEDIF(C36,D36,"d")+1</f>
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G36" s="22">
         <v>0</v>
       </c>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="12.75"/>
-    <row r="38" spans="1:8" ht="12.75">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:8" ht="12.75">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:8" ht="12.75">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:8" ht="12.75"/>
+    <row r="37" spans="1:8" ht="15">
+      <c r="A37" s="24"/>
+      <c r="B37" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="25">
+        <v>43826</v>
+      </c>
+      <c r="D37" s="27">
+        <v>43826</v>
+      </c>
+      <c r="E37" s="16">
+        <f>INT(C37)-INT($C$9)</f>
+        <v>77</v>
+      </c>
+      <c r="F37" s="23">
+        <f>DATEDIF(C37,D37,"d")+1</f>
+        <v>1</v>
+      </c>
+      <c r="G37" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="19"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+    </row>
+    <row r="39" spans="1:8" ht="15">
+      <c r="B39" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="25">
+        <v>43827</v>
+      </c>
+      <c r="D39" s="27">
+        <v>43840</v>
+      </c>
+      <c r="E39" s="16">
+        <f t="shared" ref="E39:E40" si="10">INT(C39)-INT($C$9)</f>
+        <v>78</v>
+      </c>
+      <c r="F39" s="23">
+        <f>DATEDIF(C39,D39,"d")+1</f>
+        <v>14</v>
+      </c>
+      <c r="G39" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15">
+      <c r="A40" s="30"/>
+      <c r="B40" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="25">
+        <v>43839</v>
+      </c>
+      <c r="D40" s="27">
+        <v>43840</v>
+      </c>
+      <c r="E40" s="16">
+        <f t="shared" si="10"/>
+        <v>90</v>
+      </c>
+      <c r="F40" s="23">
+        <f>DATEDIF(C40,D40,"d")+1</f>
+        <v>2</v>
+      </c>
+      <c r="G40" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15">
+      <c r="B41" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="25">
+        <v>43840</v>
+      </c>
+      <c r="D41" s="27">
+        <v>43840</v>
+      </c>
+      <c r="E41" s="16">
+        <f>INT(C41)-INT($C$9)</f>
+        <v>91</v>
+      </c>
+      <c r="F41" s="23">
+        <f>DATEDIF(C41,D41,"d")+1</f>
+        <v>1</v>
+      </c>
+      <c r="G41" s="22">
+        <v>0</v>
+      </c>
+    </row>
     <row r="42" spans="1:8" ht="15">
-      <c r="B42" s="15"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="27"/>
+      <c r="B42" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="25">
+        <v>43841</v>
+      </c>
+      <c r="D42" s="27">
+        <v>43860</v>
+      </c>
+      <c r="E42" s="16">
+        <f>INT(C42)-INT($C$9)</f>
+        <v>92</v>
+      </c>
+      <c r="F42" s="23">
+        <f>DATEDIF(C42,D42,"d")+1</f>
+        <v>20</v>
+      </c>
+      <c r="G42" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:8" ht="15">
       <c r="B43" s="15"/>
@@ -2346,6 +2628,12 @@
     <row r="50" ht="12.75"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AH6:AL6"/>
+    <mergeCell ref="AC6:AG6"/>
+    <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="S6:W6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="N6:R6"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="E6:E7"/>
@@ -2354,14 +2642,8 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="AH6:AL6"/>
-    <mergeCell ref="AC6:AG6"/>
-    <mergeCell ref="X6:AB6"/>
-    <mergeCell ref="S6:W6"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="N6:R6"/>
   </mergeCells>
-  <conditionalFormatting sqref="G34:G36 G33:H33 G9:G14 G25:G31 G16:G23">
+  <conditionalFormatting sqref="G39:G42 H33 G9:G14 G16:G23 G25:G37">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="percent" val="0"/>
@@ -2372,7 +2654,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C9:D14 D25:D31 D42:D44 D16:D23 C33:D35 C36:D36" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="D43:D44 C39:D42 D25:D37 C9:D14 D21 D16:D20 D22:D23" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>OR(NOT(ISERROR(DATEVALUE(C9))), AND(ISNUMBER(C9), LEFT(CELL("format", C9))="D"))</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>